<commit_message>
added auto computation of job cluster depending of file size
</commit_message>
<xml_diff>
--- a/dbx/dbx_schema.xlsx
+++ b/dbx/dbx_schema.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\DATA-BRICKS\SAMPLE\DBX_GENERATOR\dbx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7721AB-D00F-48E7-B0B1-ECFED8FBDB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDF9DB-AB1F-43A5-9775-2F5557E09416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="context_parameters" sheetId="2" r:id="rId2"/>
-    <sheet name="hash" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="9" r:id="rId4"/>
-    <sheet name="masking_fields" sheetId="4" r:id="rId5"/>
-    <sheet name="MASKING-GUIDE" sheetId="5" r:id="rId6"/>
+    <sheet name="jobcluster_compute" sheetId="10" r:id="rId3"/>
+    <sheet name="hash" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="9" r:id="rId5"/>
+    <sheet name="masking_fields" sheetId="4" r:id="rId6"/>
+    <sheet name="MASKING-GUIDE" sheetId="5" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="180">
   <si>
     <t>iteration</t>
   </si>
@@ -145,9 +146,6 @@
     <t>wde</t>
   </si>
   <si>
-    <t>csv</t>
-  </si>
-  <si>
     <t>p_source_directory</t>
   </si>
   <si>
@@ -508,88 +506,127 @@
     <t>file_name</t>
   </si>
   <si>
+    <t>append</t>
+  </si>
+  <si>
+    <t>Ventas - Activation CA</t>
+  </si>
+  <si>
+    <t>/talend_prod/data/hive/gdm_landing/wi_topup_converted_hly</t>
+  </si>
+  <si>
+    <t>TOPUP_CONVERTED</t>
+  </si>
+  <si>
+    <t>txn_date</t>
+  </si>
+  <si>
+    <t>effective_hour</t>
+  </si>
+  <si>
+    <t>effective_time_key</t>
+  </si>
+  <si>
+    <t>effective_dttm</t>
+  </si>
+  <si>
+    <t>aparty_loc_info</t>
+  </si>
+  <si>
+    <t>aparty_lac_info</t>
+  </si>
+  <si>
+    <t>aparty_ci_info</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>subbrand</t>
+  </si>
+  <si>
+    <t>mnp_type</t>
+  </si>
+  <si>
+    <t>source_brand</t>
+  </si>
+  <si>
+    <t>activation_dttm</t>
+  </si>
+  <si>
+    <t>usage_dttm</t>
+  </si>
+  <si>
+    <t>usage_rnk</t>
+  </si>
+  <si>
+    <t>iccid</t>
+  </si>
+  <si>
+    <t>material_code</t>
+  </si>
+  <si>
+    <t>tac</t>
+  </si>
+  <si>
+    <t>process_dttm</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>wi_topup_converted_hly</t>
-  </si>
-  <si>
-    <t>silver</t>
-  </si>
-  <si>
-    <t>cu</t>
+    <t>bronze</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>parquet</t>
+  </si>
+  <si>
+    <t>wi_topup_loaded_sync</t>
+  </si>
+  <si>
+    <t>File Format</t>
+  </si>
+  <si>
+    <t>Size (GB)</t>
+  </si>
+  <si>
+    <t>Node Type</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>≤ 5</t>
+  </si>
+  <si>
+    <t>r5.2xlarge</t>
+  </si>
+  <si>
+    <t>&gt; 5</t>
+  </si>
+  <si>
+    <t>Parquet</t>
+  </si>
+  <si>
+    <t>i3.xlarge</t>
+  </si>
+  <si>
+    <t>p_file_size</t>
+  </si>
+  <si>
+    <t>1gb</t>
   </si>
   <si>
     <t>|</t>
-  </si>
-  <si>
-    <t>append</t>
-  </si>
-  <si>
-    <t>Ventas - Activation CA</t>
-  </si>
-  <si>
-    <t>/talend_prod/data/hive/gdm_landing/wi_topup_converted_hly</t>
-  </si>
-  <si>
-    <t>TOPUP_CONVERTED</t>
-  </si>
-  <si>
-    <t>txn_date</t>
-  </si>
-  <si>
-    <t>effective_hour</t>
-  </si>
-  <si>
-    <t>effective_time_key</t>
-  </si>
-  <si>
-    <t>effective_dttm</t>
-  </si>
-  <si>
-    <t>aparty_loc_info</t>
-  </si>
-  <si>
-    <t>aparty_lac_info</t>
-  </si>
-  <si>
-    <t>aparty_ci_info</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>subbrand</t>
-  </si>
-  <si>
-    <t>mnp_type</t>
-  </si>
-  <si>
-    <t>source_brand</t>
-  </si>
-  <si>
-    <t>activation_dttm</t>
-  </si>
-  <si>
-    <t>usage_dttm</t>
-  </si>
-  <si>
-    <t>usage_rnk</t>
-  </si>
-  <si>
-    <t>iccid</t>
-  </si>
-  <si>
-    <t>material_code</t>
-  </si>
-  <si>
-    <t>tac</t>
-  </si>
-  <si>
-    <t>process_dttm</t>
-  </si>
-  <si>
-    <t>int</t>
   </si>
 </sst>
 </file>
@@ -847,7 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -928,6 +965,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,8 +1131,8 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>1234440</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1558,7 +1598,7 @@
   <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1569,7 +1609,7 @@
     <col min="4" max="4" width="8.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1584,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1593,23 +1633,23 @@
         <v>_c0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="29"/>
       <c r="I2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1618,7 +1658,7 @@
         <v>_c1</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1632,10 +1672,10 @@
         <v>_c2</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D4" s="28"/>
     </row>
@@ -1645,18 +1685,12 @@
         <v>_c3</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D5" s="28"/>
-      <c r="I5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J5" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
@@ -1664,17 +1698,17 @@
         <v>_c4</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D6" s="28"/>
       <c r="I6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1683,14 +1717,14 @@
         <v>_c5</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="28"/>
       <c r="I7" t="s">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
@@ -1702,12 +1736,18 @@
         <v>_c6</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="28"/>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
@@ -1715,7 +1755,7 @@
         <v>_c7</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1728,7 +1768,7 @@
         <v>_c8</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1741,7 +1781,7 @@
         <v>_c9</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1754,7 +1794,7 @@
         <v>_c10</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1767,7 +1807,7 @@
         <v>_c11</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -1780,10 +1820,10 @@
         <v>_c12</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="28"/>
     </row>
@@ -1793,10 +1833,10 @@
         <v>_c13</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D15" s="28"/>
     </row>
@@ -1806,10 +1846,10 @@
         <v>_c14</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D16" s="28"/>
     </row>
@@ -1819,7 +1859,7 @@
         <v>_c15</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1832,7 +1872,7 @@
         <v>_c16</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1845,7 +1885,7 @@
         <v>_c17</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1858,10 +1898,10 @@
         <v>_c18</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="28"/>
     </row>
@@ -1871,10 +1911,10 @@
         <v>_c19</v>
       </c>
       <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
         <v>137</v>
-      </c>
-      <c r="C21" t="s">
-        <v>138</v>
       </c>
       <c r="D21" s="28"/>
     </row>
@@ -1884,7 +1924,7 @@
         <v>_c20</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -2405,7 +2445,7 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="str">
-        <f t="shared" ref="A98:A129" si="3">IF(B98&lt;&gt;"", "_c" &amp; ROW(B98)-ROW($B$2), "")</f>
+        <f t="shared" ref="A98:A99" si="3">IF(B98&lt;&gt;"", "_c" &amp; ROW(B98)-ROW($B$2), "")</f>
         <v/>
       </c>
     </row>
@@ -2483,8 +2523,8 @@
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>1234440</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2528,10 +2568,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B941C014-D242-4EA1-B3FC-C880CA20A1D9}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2551,14 +2591,15 @@
     <col min="13" max="13" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.09765625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -2570,7 +2611,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -2594,58 +2635,64 @@
         <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>IF(E2="silver","_s",IF(E2="bronze","_b",IF(E2="reference"," ","")))</f>
-        <v>_s</v>
+        <v>_b</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="H2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="O2" s="5" t="s">
-        <v>148</v>
+        <v>142</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2655,6 +2702,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6512B182-C30C-4E2F-8666-FEBB2BFC77CB}">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.69921875" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="14.796875" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="39">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E990EE4C-EB41-42AA-A164-70046E99E424}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D182"/>
@@ -2679,10 +2817,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5497,7 +5635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA0B832-B55C-4960-956D-9D6CED85463F}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:Z4"/>
@@ -5536,76 +5674,76 @@
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>109</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>110</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>111</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>112</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>113</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>115</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>116</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>117</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>118</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>119</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>120</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>121</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>122</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>123</v>
       </c>
       <c r="Z1" t="s">
         <v>5</v>
@@ -5616,7 +5754,7 @@
         <v>9294029694</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5628,28 +5766,28 @@
         <v>140.166666666666</v>
       </c>
       <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" t="s">
         <v>125</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
       </c>
       <c r="K2">
         <v>2.0100000020001402E+17</v>
       </c>
       <c r="L2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M2">
         <v>2.0100000070064301E+17</v>
       </c>
       <c r="N2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O2">
         <v>2.0100000070123299E+17</v>
       </c>
       <c r="P2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q2">
         <v>2197</v>
@@ -5678,7 +5816,7 @@
         <v>9438742187</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -5690,22 +5828,22 @@
         <v>112.8</v>
       </c>
       <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" t="s">
         <v>125</v>
       </c>
-      <c r="J3" t="s">
-        <v>126</v>
-      </c>
       <c r="Q3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U3">
         <v>2025</v>
@@ -5722,7 +5860,7 @@
         <v>9081374265</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -5734,28 +5872,28 @@
         <v>73.2</v>
       </c>
       <c r="H4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" t="s">
         <v>125</v>
-      </c>
-      <c r="J4" t="s">
-        <v>126</v>
       </c>
       <c r="K4">
         <v>2.01000000200016E+17</v>
       </c>
       <c r="L4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M4">
         <v>2.0100000020000998E+17</v>
       </c>
       <c r="N4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O4">
         <v>2.0100000020002499E+17</v>
       </c>
       <c r="P4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q4">
         <v>2041</v>
@@ -5784,7 +5922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A88009-93D8-4B0A-8C70-440B2F9898E3}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I100"/>
@@ -5805,22 +5943,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I1" s="1">
         <v>9</v>
@@ -5832,20 +5970,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>26</v>
-      </c>
       <c r="D2" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="22" t="str">
         <f>IF(B2&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B2)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B2), INDEX($I$2:$I$15, MATCH(B2, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(owning_subscriber_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as owning_subscriber_id</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="21" t="str" cm="1">
         <f t="array" ref="I2">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H2)</f>
@@ -5861,10 +5999,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="22" t="str">
         <f>IF(B3&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B3)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B3), INDEX($I$2:$I$15, MATCH(B3, $H$2:$H$15, 0))),"")</f>
@@ -5884,20 +6022,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="22" t="str">
         <f>IF(B4&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B4)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B4), INDEX($I$2:$I$15, MATCH(B4, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(subscriber_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as subscriber_id</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="21" t="str" cm="1">
         <f t="array" ref="I4">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H4)</f>
@@ -5910,20 +6048,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="22" t="str">
         <f>IF(B5&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B5)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B5), INDEX($I$2:$I$15, MATCH(B5, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(retailer_id), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as retailer_id</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="21" t="str" cm="1">
         <f t="array" ref="I5">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H5)</f>
@@ -5936,20 +6074,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="22" t="str">
         <f>IF(B6&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B6)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B6), INDEX($I$2:$I$15, MATCH(B6, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(ret_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_id</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I6" s="21" t="str" cm="1">
         <f t="array" ref="I6">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H6)</f>
@@ -5962,20 +6100,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="22" t="str">
         <f>IF(B7&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B7)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B7), INDEX($I$2:$I$15, MATCH(B7, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(sub_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as sub_id</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="21" t="str" cm="1">
         <f t="array" ref="I7">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H7)</f>
@@ -5988,20 +6126,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="22" t="str">
         <f>IF(B8&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B8)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B8), INDEX($I$2:$I$15, MATCH(B8, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(fund_src), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as fund_src</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="21" t="str" cm="1">
         <f t="array" ref="I8">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H8)</f>
@@ -6014,20 +6152,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="22" t="str">
         <f>IF(B9&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B9)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B9), INDEX($I$2:$I$15, MATCH(B9, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(imsi), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as imsi</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9" s="21" t="str" cm="1">
         <f t="array" ref="I9">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H9)</f>
@@ -6040,20 +6178,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="22" t="str">
         <f>IF(B10&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B10)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B10), INDEX($I$2:$I$15, MATCH(B10, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(callingnumber), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as callingnumber</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="21" t="str" cm="1">
         <f t="array" ref="I10">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H10)</f>
@@ -6066,20 +6204,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="22" t="str">
         <f>IF(B11&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B11)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B11), INDEX($I$2:$I$15, MATCH(B11, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(callednumber), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as callednumber</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I11" s="21" t="str" cm="1">
         <f t="array" ref="I11">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H11)</f>
@@ -6092,20 +6230,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="22" t="str">
         <f>IF(B12&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B12)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B12), INDEX($I$2:$I$15, MATCH(B12, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(ret_min as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_min</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="21" t="str" cm="1">
         <f t="array" ref="I12">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H12)</f>
@@ -6118,20 +6256,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="22" t="str">
         <f>IF(B13&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B13)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B13), INDEX($I$2:$I$15, MATCH(B13, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(ret_msisdn as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_msisdn</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="21" t="str" cm="1">
         <f t="array" ref="I13">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H13)</f>
@@ -6144,20 +6282,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="22" t="str">
         <f>IF(B14&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B14)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B14), INDEX($I$2:$I$15, MATCH(B14, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(imei), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as imei</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I14" s="21" t="str" cm="1">
         <f t="array" ref="I14">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H14)</f>
@@ -6170,20 +6308,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="22" t="str">
         <f>IF(B15&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B15)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B15), INDEX($I$2:$I$15, MATCH(B15, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat('63', trim(cast(dsp_min as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as dsp_min</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I15" s="21" t="str" cm="1">
         <f t="array" ref="I15">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H15)</f>
@@ -6196,13 +6334,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="22" t="str">
         <f>IF(B16&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B16)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B16), INDEX($I$2:$I$15, MATCH(B16, $H$2:$H$15, 0))),"")</f>
@@ -6215,13 +6353,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="22" t="str">
         <f>IF(B17&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B17)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B17), INDEX($I$2:$I$15, MATCH(B17, $H$2:$H$15, 0))),"")</f>
@@ -6234,13 +6372,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="22" t="str">
         <f>IF(B18&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B18)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B18), INDEX($I$2:$I$15, MATCH(B18, $H$2:$H$15, 0))),"")</f>
@@ -6253,13 +6391,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="22" t="str">
         <f>IF(B19&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B19)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B19), INDEX($I$2:$I$15, MATCH(B19, $H$2:$H$15, 0))),"")</f>
@@ -6272,13 +6410,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="22" t="str">
         <f>IF(B20&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B20)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B20), INDEX($I$2:$I$15, MATCH(B20, $H$2:$H$15, 0))),"")</f>
@@ -6291,13 +6429,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="22" t="str">
         <f>IF(B21&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B21)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B21), INDEX($I$2:$I$15, MATCH(B21, $H$2:$H$15, 0))),"")</f>
@@ -6310,13 +6448,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="22" t="str">
         <f>IF(B22&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B22)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B22), INDEX($I$2:$I$15, MATCH(B22, $H$2:$H$15, 0))),"")</f>
@@ -6329,13 +6467,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="22" t="str">
         <f>IF(B23&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B23)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B23), INDEX($I$2:$I$15, MATCH(B23, $H$2:$H$15, 0))),"")</f>
@@ -6348,13 +6486,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="22" t="str">
         <f>IF(B24&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B24)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B24), INDEX($I$2:$I$15, MATCH(B24, $H$2:$H$15, 0))),"")</f>
@@ -6367,13 +6505,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="22" t="str">
         <f>IF(B25&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B25)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B25), INDEX($I$2:$I$15, MATCH(B25, $H$2:$H$15, 0))),"")</f>
@@ -6386,13 +6524,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E26" s="22" t="str">
         <f>IF(B26&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B26)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B26), INDEX($I$2:$I$15, MATCH(B26, $H$2:$H$15, 0))),"")</f>
@@ -6405,13 +6543,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" s="22" t="str">
         <f>IF(B27&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B27)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B27), INDEX($I$2:$I$15, MATCH(B27, $H$2:$H$15, 0))),"")</f>
@@ -6424,13 +6562,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="22" t="str">
         <f>IF(B28&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B28)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B28), INDEX($I$2:$I$15, MATCH(B28, $H$2:$H$15, 0))),"")</f>
@@ -6443,13 +6581,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" s="22" t="str">
         <f>IF(B29&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B29)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B29), INDEX($I$2:$I$15, MATCH(B29, $H$2:$H$15, 0))),"")</f>
@@ -6462,13 +6600,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="22" t="str">
         <f>IF(B30&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B30)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B30), INDEX($I$2:$I$15, MATCH(B30, $H$2:$H$15, 0))),"")</f>
@@ -6481,13 +6619,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="22" t="str">
         <f>IF(B31&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B31)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B31), INDEX($I$2:$I$15, MATCH(B31, $H$2:$H$15, 0))),"")</f>
@@ -6500,13 +6638,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="22" t="str">
         <f>IF(B32&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B32)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B32), INDEX($I$2:$I$15, MATCH(B32, $H$2:$H$15, 0))),"")</f>
@@ -6519,13 +6657,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="22" t="str">
         <f>IF(B33&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B33)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B33), INDEX($I$2:$I$15, MATCH(B33, $H$2:$H$15, 0))),"")</f>
@@ -6538,13 +6676,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="22" t="str">
         <f>IF(B34&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B34)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B34), INDEX($I$2:$I$15, MATCH(B34, $H$2:$H$15, 0))),"")</f>
@@ -6557,13 +6695,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E35" s="22" t="str">
         <f>IF(B35&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B35)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B35), INDEX($I$2:$I$15, MATCH(B35, $H$2:$H$15, 0))),"")</f>
@@ -6579,10 +6717,10 @@
         <v>4</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="22" t="str">
         <f>IF(B36&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B36)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B36), INDEX($I$2:$I$15, MATCH(B36, $H$2:$H$15, 0))),"")</f>
@@ -6595,13 +6733,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" s="22" t="str">
         <f>IF(B37&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B37)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B37), INDEX($I$2:$I$15, MATCH(B37, $H$2:$H$15, 0))),"")</f>
@@ -6614,13 +6752,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="22" t="str">
         <f>IF(B38&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B38)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B38), INDEX($I$2:$I$15, MATCH(B38, $H$2:$H$15, 0))),"")</f>
@@ -6633,13 +6771,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" s="22" t="str">
         <f>IF(B39&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B39)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B39), INDEX($I$2:$I$15, MATCH(B39, $H$2:$H$15, 0))),"")</f>
@@ -6652,13 +6790,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40" s="22" t="str">
         <f>IF(B40&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B40)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B40), INDEX($I$2:$I$15, MATCH(B40, $H$2:$H$15, 0))),"")</f>
@@ -7083,7 +7221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85241015-4B45-4A87-AF5E-CDB473B1D3F3}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K24"/>
@@ -7121,7 +7259,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -7149,7 +7287,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -7192,13 +7330,13 @@
       <c r="F7" s="10"/>
       <c r="G7" s="6"/>
       <c r="H7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="K7" s="14"/>
     </row>
@@ -7208,19 +7346,19 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="G8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="14"/>
@@ -7233,13 +7371,13 @@
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
       <c r="G9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="I9" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9" s="16" t="b">
         <v>1</v>
@@ -7265,19 +7403,19 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="G11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>76</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="14"/>
@@ -7290,13 +7428,13 @@
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
       <c r="G12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="I12" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" s="16" t="b">
         <v>1</v>
@@ -7324,7 +7462,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="6">
         <v>64</v>
@@ -7355,7 +7493,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -7398,13 +7536,13 @@
       <c r="F19" s="10"/>
       <c r="G19" s="6"/>
       <c r="H19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="J19" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -7414,19 +7552,19 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="G20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="6"/>
@@ -7439,13 +7577,13 @@
       <c r="E21" s="36"/>
       <c r="F21" s="38"/>
       <c r="G21" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J21" s="16" t="b">
         <v>1</v>
@@ -7484,7 +7622,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
fixed file name convention
</commit_message>
<xml_diff>
--- a/dbx/dbx_schema.xlsx
+++ b/dbx/dbx_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\DATA-BRICKS\SAMPLE\DBX_GENERATOR\dbx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DDF9DB-AB1F-43A5-9775-2F5557E09416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76100E1F-54D2-42D9-88D5-99EA4F81F9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="173">
   <si>
     <t>iteration</t>
   </si>
@@ -485,148 +485,127 @@
     <t>tier_suffix</t>
   </si>
   <si>
+    <t>p_local_laptop_path</t>
+  </si>
+  <si>
+    <t>C:\\AUTOMATION\\</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>dbx_process_dttm</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>File Format</t>
+  </si>
+  <si>
+    <t>Size (GB)</t>
+  </si>
+  <si>
+    <t>Node Type</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>≤ 5</t>
+  </si>
+  <si>
+    <t>r5.2xlarge</t>
+  </si>
+  <si>
+    <t>&gt; 5</t>
+  </si>
+  <si>
+    <t>Parquet</t>
+  </si>
+  <si>
+    <t>i3.xlarge</t>
+  </si>
+  <si>
+    <t>p_file_size</t>
+  </si>
+  <si>
     <t>daily</t>
   </si>
   <si>
-    <t>p_local_laptop_path</t>
-  </si>
-  <si>
-    <t>C:\\AUTOMATION\\</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>dbx_process_dttm</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>file_name</t>
-  </si>
-  <si>
-    <t>append</t>
-  </si>
-  <si>
-    <t>Ventas - Activation CA</t>
-  </si>
-  <si>
-    <t>/talend_prod/data/hive/gdm_landing/wi_topup_converted_hly</t>
-  </si>
-  <si>
-    <t>TOPUP_CONVERTED</t>
-  </si>
-  <si>
-    <t>txn_date</t>
-  </si>
-  <si>
-    <t>effective_hour</t>
-  </si>
-  <si>
-    <t>effective_time_key</t>
-  </si>
-  <si>
-    <t>effective_dttm</t>
-  </si>
-  <si>
-    <t>aparty_loc_info</t>
-  </si>
-  <si>
-    <t>aparty_lac_info</t>
-  </si>
-  <si>
-    <t>aparty_ci_info</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>subbrand</t>
-  </si>
-  <si>
-    <t>mnp_type</t>
-  </si>
-  <si>
-    <t>source_brand</t>
-  </si>
-  <si>
-    <t>activation_dttm</t>
-  </si>
-  <si>
-    <t>usage_dttm</t>
-  </si>
-  <si>
-    <t>usage_rnk</t>
-  </si>
-  <si>
-    <t>iccid</t>
-  </si>
-  <si>
-    <t>material_code</t>
-  </si>
-  <si>
-    <t>tac</t>
-  </si>
-  <si>
-    <t>process_dttm</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>bronze</t>
-  </si>
-  <si>
-    <t>pr</t>
-  </si>
-  <si>
-    <t>parquet</t>
-  </si>
-  <si>
-    <t>wi_topup_loaded_sync</t>
-  </si>
-  <si>
-    <t>File Format</t>
-  </si>
-  <si>
-    <t>Size (GB)</t>
-  </si>
-  <si>
-    <t>Node Type</t>
-  </si>
-  <si>
-    <t>Workers</t>
-  </si>
-  <si>
-    <t>CSV</t>
-  </si>
-  <si>
-    <t>≤ 5</t>
-  </si>
-  <si>
-    <t>r5.2xlarge</t>
-  </si>
-  <si>
-    <t>&gt; 5</t>
-  </si>
-  <si>
-    <t>Parquet</t>
-  </si>
-  <si>
-    <t>i3.xlarge</t>
-  </si>
-  <si>
-    <t>p_file_size</t>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>overwrite</t>
+  </si>
+  <si>
+    <t>Source Channel Reference</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>/talend_prod/data/hive/gdm_landing/sourcechannel/</t>
+  </si>
+  <si>
+    <t>SOURCECHANNEL</t>
   </si>
   <si>
     <t>1gb</t>
   </si>
   <si>
-    <t>|</t>
+    <t>decimal(30,0)</t>
+  </si>
+  <si>
+    <t>d_sourcechannel_sk</t>
+  </si>
+  <si>
+    <t>sourcechannel_cd</t>
+  </si>
+  <si>
+    <t>sourcechannel_nm</t>
+  </si>
+  <si>
+    <t>sourcechannel_desc</t>
+  </si>
+  <si>
+    <t>sourcechannel_group</t>
+  </si>
+  <si>
+    <t>sourcechannel_type</t>
+  </si>
+  <si>
+    <t>entity_cd</t>
+  </si>
+  <si>
+    <t>valid_from</t>
+  </si>
+  <si>
+    <t>valid_to</t>
+  </si>
+  <si>
+    <t>active_flag</t>
+  </si>
+  <si>
+    <t>pasaload_type</t>
+  </si>
+  <si>
+    <t>ensa_dly_cei_province</t>
+  </si>
+  <si>
+    <t>rt</t>
   </si>
 </sst>
 </file>
@@ -945,6 +924,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -965,9 +947,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1597,8 +1576,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1624,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1633,10 +1612,10 @@
         <v>_c0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="D2" s="29"/>
       <c r="I2" s="1" t="s">
@@ -1658,7 +1637,7 @@
         <v>_c1</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1672,10 +1651,10 @@
         <v>_c2</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>6</v>
       </c>
       <c r="D4" s="28"/>
     </row>
@@ -1685,10 +1664,10 @@
         <v>_c3</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>6</v>
       </c>
       <c r="D5" s="28"/>
     </row>
@@ -1698,17 +1677,17 @@
         <v>_c4</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="D6" s="28"/>
       <c r="I6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" t="s">
         <v>136</v>
-      </c>
-      <c r="J6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1717,14 +1696,14 @@
         <v>_c5</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="28"/>
       <c r="I7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
@@ -1736,7 +1715,7 @@
         <v>_c6</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1755,10 +1734,10 @@
         <v>_c7</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D9" s="28"/>
     </row>
@@ -1768,10 +1747,10 @@
         <v>_c8</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D10" s="28"/>
     </row>
@@ -1781,7 +1760,7 @@
         <v>_c9</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1794,10 +1773,10 @@
         <v>_c10</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="D12" s="28"/>
     </row>
@@ -1807,10 +1786,10 @@
         <v>_c11</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D13" s="28"/>
     </row>
@@ -1820,10 +1799,10 @@
         <v>_c12</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="D14" s="28"/>
     </row>
@@ -1833,114 +1812,66 @@
         <v>_c13</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="D15" s="28"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>_c14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" t="s">
-        <v>161</v>
+        <v/>
       </c>
       <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>_c15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>_c16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="D18" s="28"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>_c17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>159</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="D19" s="28"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>_c18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C20" t="s">
-        <v>137</v>
+        <v/>
       </c>
       <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>_c19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" t="s">
-        <v>137</v>
+        <v/>
       </c>
       <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>_c20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>_c21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="D23" s="28"/>
     </row>
@@ -2570,8 +2501,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2599,7 +2530,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -2641,7 +2572,7 @@
         <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -2649,50 +2580,50 @@
         <v>18</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>IF(E2="silver","_s",IF(E2="bronze","_b",IF(E2="reference"," ","")))</f>
-        <v>_b</v>
+        <v>_s</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" s="39" t="s">
-        <v>178</v>
+        <v>157</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2719,71 +2650,71 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3" s="39">
+        <v>145</v>
+      </c>
+      <c r="E3" s="32">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="39">
+        <v>145</v>
+      </c>
+      <c r="E4" s="32">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E5" s="39">
+        <v>148</v>
+      </c>
+      <c r="E5" s="32">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="39">
+        <v>148</v>
+      </c>
+      <c r="E6" s="32">
         <v>4</v>
       </c>
     </row>
@@ -2826,29 +2757,29 @@
     <row r="2" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(B2&lt;&gt;"", ROW(B2)-ROW($B$2) &amp; ","&amp;B2, "")</f>
-        <v>0,owning_subscriber_id</v>
+        <v>0,d_sourcechannel_sk</v>
       </c>
       <c r="B2" t="str">
         <f>IF(schema!B2&lt;&gt;"", schema!B2, "")</f>
-        <v>owning_subscriber_id</v>
+        <v>d_sourcechannel_sk</v>
       </c>
       <c r="C2" t="str">
         <f>IF(schema!C2&lt;&gt;"", schema!C2, "")</f>
-        <v>string</v>
+        <v>decimal(30,0)</v>
       </c>
       <c r="D2" s="22" t="str">
         <f>IF(schema!B2&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B2), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B2, 0),"")</f>
-        <v>lower(sha2(concat('63', trim(cast(owning_subscriber_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as owning_subscriber_id</v>
+        <v>d_sourcechannel_sk</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">IF(B3&lt;&gt;"", ROW(B3)-ROW($B$2) &amp; ","&amp;B3, "")</f>
-        <v>1,txn_date</v>
+        <v>1,sourcechannel_cd</v>
       </c>
       <c r="B3" t="str">
         <f>IF(schema!B3&lt;&gt;"", schema!B3, "")</f>
-        <v>txn_date</v>
+        <v>sourcechannel_cd</v>
       </c>
       <c r="C3" t="str">
         <f>IF(schema!C3&lt;&gt;"", schema!C3, "")</f>
@@ -2856,71 +2787,71 @@
       </c>
       <c r="D3" s="22" t="str">
         <f>IF(schema!B3&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B3), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B3, 0),"")</f>
-        <v>txn_date</v>
+        <v>sourcechannel_cd</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>2,effective_hour</v>
+        <v>2,sourcechannel_nm</v>
       </c>
       <c r="B4" t="str">
         <f>IF(schema!B4&lt;&gt;"", schema!B4, "")</f>
-        <v>effective_hour</v>
+        <v>sourcechannel_nm</v>
       </c>
       <c r="C4" t="str">
         <f>IF(schema!C4&lt;&gt;"", schema!C4, "")</f>
-        <v>int</v>
+        <v>string</v>
       </c>
       <c r="D4" s="22" t="str">
         <f>IF(schema!B4&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B4), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B4, 0),"")</f>
-        <v>effective_hour</v>
+        <v>sourcechannel_nm</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>3,effective_time_key</v>
+        <v>3,sourcechannel_desc</v>
       </c>
       <c r="B5" t="str">
         <f>IF(schema!B5&lt;&gt;"", schema!B5, "")</f>
-        <v>effective_time_key</v>
+        <v>sourcechannel_desc</v>
       </c>
       <c r="C5" t="str">
         <f>IF(schema!C5&lt;&gt;"", schema!C5, "")</f>
-        <v>int</v>
+        <v>string</v>
       </c>
       <c r="D5" s="22" t="str">
         <f>IF(schema!B5&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B5), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B5, 0),"")</f>
-        <v>effective_time_key</v>
+        <v>sourcechannel_desc</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>4,effective_dttm</v>
+        <v>4,sourcechannel_group</v>
       </c>
       <c r="B6" t="str">
         <f>IF(schema!B6&lt;&gt;"", schema!B6, "")</f>
-        <v>effective_dttm</v>
+        <v>sourcechannel_group</v>
       </c>
       <c r="C6" t="str">
         <f>IF(schema!C6&lt;&gt;"", schema!C6, "")</f>
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="D6" s="22" t="str">
         <f>IF(schema!B6&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B6), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B6, 0),"")</f>
-        <v>effective_dttm</v>
+        <v>sourcechannel_group</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>5,aparty_loc_info</v>
+        <v>5,sourcechannel_type</v>
       </c>
       <c r="B7" t="str">
         <f>IF(schema!B7&lt;&gt;"", schema!B7, "")</f>
-        <v>aparty_loc_info</v>
+        <v>sourcechannel_type</v>
       </c>
       <c r="C7" t="str">
         <f>IF(schema!C7&lt;&gt;"", schema!C7, "")</f>
@@ -2928,17 +2859,17 @@
       </c>
       <c r="D7" s="22" t="str">
         <f>IF(schema!B7&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B7), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B7, 0),"")</f>
-        <v>aparty_loc_info</v>
+        <v>sourcechannel_type</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>6,aparty_lac_info</v>
+        <v>6,entity_cd</v>
       </c>
       <c r="B8" t="str">
         <f>IF(schema!B8&lt;&gt;"", schema!B8, "")</f>
-        <v>aparty_lac_info</v>
+        <v>entity_cd</v>
       </c>
       <c r="C8" t="str">
         <f>IF(schema!C8&lt;&gt;"", schema!C8, "")</f>
@@ -2946,53 +2877,53 @@
       </c>
       <c r="D8" s="22" t="str">
         <f>IF(schema!B8&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B8), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B8, 0),"")</f>
-        <v>aparty_lac_info</v>
+        <v>entity_cd</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>7,aparty_ci_info</v>
+        <v>7,valid_from</v>
       </c>
       <c r="B9" t="str">
         <f>IF(schema!B9&lt;&gt;"", schema!B9, "")</f>
-        <v>aparty_ci_info</v>
+        <v>valid_from</v>
       </c>
       <c r="C9" t="str">
         <f>IF(schema!C9&lt;&gt;"", schema!C9, "")</f>
-        <v>string</v>
+        <v>timestamp</v>
       </c>
       <c r="D9" s="22" t="str">
         <f>IF(schema!B9&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B9), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B9, 0),"")</f>
-        <v>aparty_ci_info</v>
+        <v>valid_from</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>8,brand</v>
+        <v>8,valid_to</v>
       </c>
       <c r="B10" t="str">
         <f>IF(schema!B10&lt;&gt;"", schema!B10, "")</f>
-        <v>brand</v>
+        <v>valid_to</v>
       </c>
       <c r="C10" t="str">
         <f>IF(schema!C10&lt;&gt;"", schema!C10, "")</f>
-        <v>string</v>
+        <v>timestamp</v>
       </c>
       <c r="D10" s="22" t="str">
         <f>IF(schema!B10&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B10), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B10, 0),"")</f>
-        <v>brand</v>
+        <v>valid_to</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>9,subbrand</v>
+        <v>9,active_flag</v>
       </c>
       <c r="B11" t="str">
         <f>IF(schema!B11&lt;&gt;"", schema!B11, "")</f>
-        <v>subbrand</v>
+        <v>active_flag</v>
       </c>
       <c r="C11" t="str">
         <f>IF(schema!C11&lt;&gt;"", schema!C11, "")</f>
@@ -3000,223 +2931,223 @@
       </c>
       <c r="D11" s="22" t="str">
         <f>IF(schema!B11&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B11), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B11, 0),"")</f>
-        <v>subbrand</v>
+        <v>active_flag</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>10,mnp_type</v>
+        <v>10,pasaload_type</v>
       </c>
       <c r="B12" t="str">
         <f>IF(schema!B12&lt;&gt;"", schema!B12, "")</f>
-        <v>mnp_type</v>
+        <v>pasaload_type</v>
       </c>
       <c r="C12" t="str">
         <f>IF(schema!C12&lt;&gt;"", schema!C12, "")</f>
-        <v>string</v>
+        <v>decimal(30,0)</v>
       </c>
       <c r="D12" s="22" t="str">
         <f>IF(schema!B12&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B12), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B12, 0),"")</f>
-        <v>mnp_type</v>
+        <v>pasaload_type</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>11,source_brand</v>
+        <v>11,dbx_process_dttm</v>
       </c>
       <c r="B13" t="str">
         <f>IF(schema!B13&lt;&gt;"", schema!B13, "")</f>
-        <v>source_brand</v>
+        <v>dbx_process_dttm</v>
       </c>
       <c r="C13" t="str">
         <f>IF(schema!C13&lt;&gt;"", schema!C13, "")</f>
-        <v>string</v>
+        <v>timestamp</v>
       </c>
       <c r="D13" s="22" t="str">
         <f>IF(schema!B13&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B13), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B13, 0),"")</f>
-        <v>source_brand</v>
+        <v>dbx_process_dttm</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>12,activation_dttm</v>
+        <v>12,file_name</v>
       </c>
       <c r="B14" t="str">
         <f>IF(schema!B14&lt;&gt;"", schema!B14, "")</f>
-        <v>activation_dttm</v>
+        <v>file_name</v>
       </c>
       <c r="C14" t="str">
         <f>IF(schema!C14&lt;&gt;"", schema!C14, "")</f>
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="D14" s="22" t="str">
         <f>IF(schema!B14&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B14), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B14, 0),"")</f>
-        <v>activation_dttm</v>
+        <v>file_name</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>13,usage_dttm</v>
+        <v>13,file_id</v>
       </c>
       <c r="B15" t="str">
         <f>IF(schema!B15&lt;&gt;"", schema!B15, "")</f>
-        <v>usage_dttm</v>
+        <v>file_id</v>
       </c>
       <c r="C15" t="str">
         <f>IF(schema!C15&lt;&gt;"", schema!C15, "")</f>
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="D15" s="22" t="str">
         <f>IF(schema!B15&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B15), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B15, 0),"")</f>
-        <v>usage_dttm</v>
+        <v>file_id</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>14,usage_rnk</v>
+        <v/>
       </c>
       <c r="B16" t="str">
         <f>IF(schema!B16&lt;&gt;"", schema!B16, "")</f>
-        <v>usage_rnk</v>
+        <v/>
       </c>
       <c r="C16" t="str">
         <f>IF(schema!C16&lt;&gt;"", schema!C16, "")</f>
-        <v>int</v>
+        <v/>
       </c>
       <c r="D16" s="22" t="str">
         <f>IF(schema!B16&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B16), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B16, 0),"")</f>
-        <v>usage_rnk</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>15,iccid</v>
+        <v/>
       </c>
       <c r="B17" t="str">
         <f>IF(schema!B17&lt;&gt;"", schema!B17, "")</f>
-        <v>iccid</v>
+        <v/>
       </c>
       <c r="C17" t="str">
         <f>IF(schema!C17&lt;&gt;"", schema!C17, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D17" s="22" t="str">
         <f>IF(schema!B17&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B17), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B17, 0),"")</f>
-        <v>iccid</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>16,material_code</v>
+        <v/>
       </c>
       <c r="B18" t="str">
         <f>IF(schema!B18&lt;&gt;"", schema!B18, "")</f>
-        <v>material_code</v>
+        <v/>
       </c>
       <c r="C18" t="str">
         <f>IF(schema!C18&lt;&gt;"", schema!C18, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D18" s="22" t="str">
         <f>IF(schema!B18&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B18), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B18, 0),"")</f>
-        <v>material_code</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>17,tac</v>
+        <v/>
       </c>
       <c r="B19" t="str">
         <f>IF(schema!B19&lt;&gt;"", schema!B19, "")</f>
-        <v>tac</v>
+        <v/>
       </c>
       <c r="C19" t="str">
         <f>IF(schema!C19&lt;&gt;"", schema!C19, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D19" s="22" t="str">
         <f>IF(schema!B19&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B19), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B19, 0),"")</f>
-        <v>tac</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:4" s="23" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>18,process_dttm</v>
+        <v/>
       </c>
       <c r="B20" s="23" t="str">
         <f>IF(schema!B20&lt;&gt;"", schema!B20, "")</f>
-        <v>process_dttm</v>
+        <v/>
       </c>
       <c r="C20" s="23" t="str">
         <f>IF(schema!C20&lt;&gt;"", schema!C20, "")</f>
-        <v>timestamp</v>
+        <v/>
       </c>
       <c r="D20" s="22" t="str">
         <f>IF(schema!B20&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B20), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B20, 0),"")</f>
-        <v>process_dttm</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:4" s="23" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>19,dbx_process_dttm</v>
+        <v/>
       </c>
       <c r="B21" s="23" t="str">
         <f>IF(schema!B21&lt;&gt;"", schema!B21, "")</f>
-        <v>dbx_process_dttm</v>
+        <v/>
       </c>
       <c r="C21" s="23" t="str">
         <f>IF(schema!C21&lt;&gt;"", schema!C21, "")</f>
-        <v>timestamp</v>
+        <v/>
       </c>
       <c r="D21" s="22" t="str">
         <f>IF(schema!B21&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B21), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B21, 0),"")</f>
-        <v>dbx_process_dttm</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:4" s="23" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>20,file_name</v>
+        <v/>
       </c>
       <c r="B22" s="23" t="str">
         <f>IF(schema!B22&lt;&gt;"", schema!B22, "")</f>
-        <v>file_name</v>
+        <v/>
       </c>
       <c r="C22" s="23" t="str">
         <f>IF(schema!C22&lt;&gt;"", schema!C22, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D22" s="22" t="str">
         <f>IF(schema!B22&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B22), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B22, 0),"")</f>
-        <v>file_name</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:4" s="23" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>21,file_id</v>
+        <v/>
       </c>
       <c r="B23" s="23" t="str">
         <f>IF(schema!B23&lt;&gt;"", schema!B23, "")</f>
-        <v>file_id</v>
+        <v/>
       </c>
       <c r="C23" s="23" t="str">
         <f>IF(schema!C23&lt;&gt;"", schema!C23, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D23" s="22" t="str">
         <f>IF(schema!B23&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B23), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B23, 0),"")</f>
-        <v>file_id</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:4" s="23" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7345,10 +7276,10 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="36" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -7368,8 +7299,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="13" t="s">
         <v>71</v>
       </c>
@@ -7402,10 +7333,10 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="36" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -7425,8 +7356,8 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="13" t="s">
         <v>71</v>
       </c>
@@ -7551,10 +7482,10 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="38" t="s">
         <v>80</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -7574,8 +7505,8 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="38"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="13" t="s">
         <v>71</v>
       </c>
@@ -7621,14 +7552,14 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="35"/>
       <c r="K24" s="6"/>
     </row>
   </sheetData>

</xml_diff>